<commit_message>
Delete duplicates function added
</commit_message>
<xml_diff>
--- a/사실관계 정리표.xlsx
+++ b/사실관계 정리표.xlsx
@@ -472,7 +472,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -495,7 +495,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>(19.03.12)답변서</t>
+          <t>(19.03.12)</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -518,7 +518,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(19.03.12)답변서</t>
+          <t>(19.03.12)</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -541,7 +541,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>(19.03.12)답변서</t>
+          <t>(19.03.12)</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -564,7 +564,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>(19.03.12)답변서</t>
+          <t>(19.03.12)</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -587,7 +587,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -610,7 +610,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -633,7 +633,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>(19.01.29)소장</t>
+          <t>(19.01.29)</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -656,7 +656,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -679,7 +679,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>(19.01.29)소장</t>
+          <t>(19.01.29)</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -702,7 +702,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>(19.03.12)답변서</t>
+          <t>(19.03.12)</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -725,7 +725,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>(19.03.12)답변서</t>
+          <t>(19.03.12)</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -748,7 +748,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -771,7 +771,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>(19.03.12)답변서</t>
+          <t>(19.03.12)</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -794,7 +794,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>(19.03.12)답변서</t>
+          <t>(19.03.12)</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -817,7 +817,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -840,7 +840,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -863,7 +863,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>(19.01.29)소장</t>
+          <t>(19.01.29)</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -886,7 +886,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>(19.03.12)답변서</t>
+          <t>(19.03.12)</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -909,7 +909,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>(19.03.12)답변서</t>
+          <t>(19.03.12)</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -932,7 +932,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -955,7 +955,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -978,7 +978,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>(19.03.12)답변서</t>
+          <t>(19.03.12)</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1047,7 +1047,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1070,7 +1070,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>(19.01.29)소장</t>
+          <t>(19.01.29)</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>(19.01.29)소장</t>
+          <t>(19.01.29)</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>(19.01.29)소장</t>
+          <t>(19.01.29)</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1139,7 +1139,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>(19.01.29)소장</t>
+          <t>(19.01.29)</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1162,7 +1162,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>(19.01.29)소장</t>
+          <t>(19.01.29)</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1185,7 +1185,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>(19.01.29)소장</t>
+          <t>(19.01.29)</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>(19.03.12)답변서</t>
+          <t>(19.03.12)</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>(19.03.12)답변서</t>
+          <t>(19.03.12)</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1277,7 +1277,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1323,7 +1323,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>(19.01.29)소장</t>
+          <t>(19.01.29)</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>(19.01.29)소장</t>
+          <t>(19.01.29)</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1369,7 +1369,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>(19.01.29)소장</t>
+          <t>(19.01.29)</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1392,7 +1392,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>(19.01.29)소장</t>
+          <t>(19.01.29)</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1415,7 +1415,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>(19.03.12)답변서</t>
+          <t>(19.03.12)</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>(19.03.12)답변서</t>
+          <t>(19.03.12)</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1484,7 +1484,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1507,7 +1507,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1530,7 +1530,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>(19.01.29)소장</t>
+          <t>(19.01.29)</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>(19.03.12)답변서</t>
+          <t>(19.03.12)</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>(19.04.25)답변서</t>
+          <t>(19.04.25)</t>
         </is>
       </c>
       <c r="D50" t="n">

</xml_diff>